<commit_message>
Append Data Code Drafted
</commit_message>
<xml_diff>
--- a/Football Club Stats.zip_unzipped/Football Club Stats/Arsenal Stats.xlsx
+++ b/Football Club Stats.zip_unzipped/Football Club Stats/Arsenal Stats.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/61d616e511083e6c/Documents/Uni/Module 2- Digital Maths and Programming/Uni-Assignment/Uni-Assignment/Football Club Stats.zip_unzipped/Football Club Stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{85357D8D-E99A-4B03-AAEA-2211DA2B466C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{85357D8D-E99A-4B03-AAEA-2211DA2B466C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{833419DF-F168-47AA-B37E-6EB2DDF6ECFD}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{53058845-DA59-4129-98B6-1ADCB8415563}"/>
   </bookViews>
   <sheets>
     <sheet name="Arsenal Stats" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Arsenal Stats'!$A$1:$A$3</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Team</t>
   </si>
@@ -81,6 +84,18 @@
   </si>
   <si>
     <t>Kai Havertz</t>
+  </si>
+  <si>
+    <t>Season</t>
+  </si>
+  <si>
+    <t>24/25</t>
+  </si>
+  <si>
+    <t>23/24</t>
+  </si>
+  <si>
+    <t>Bukayo Saka</t>
   </si>
 </sst>
 </file>
@@ -158,8 +173,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DFD8BAF7-3BF3-44A3-9F78-52412893AEE2}" name="Table1" displayName="Table1" ref="A1:M2" totalsRowShown="0">
-  <autoFilter ref="A1:M2" xr:uid="{8F3199D6-65AA-43E9-A89B-2666067BF545}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DFD8BAF7-3BF3-44A3-9F78-52412893AEE2}" name="Table1" displayName="Table1" ref="B1:N3" totalsRowShown="0">
+  <autoFilter ref="B1:N3" xr:uid="{8F3199D6-65AA-43E9-A89B-2666067BF545}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{4AB07E5B-E12D-4762-8B08-9E7448195CEB}" name="Team"/>
     <tableColumn id="2" xr3:uid="{0C6E97DC-E063-40D0-9608-4C6350E2CF86}" name="Table Position"/>
@@ -496,108 +511,159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F91F743A-E395-456E-9AA7-DFC2D0CBAC97}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" customWidth="1"/>
-    <col min="4" max="4" width="15.90625" customWidth="1"/>
-    <col min="8" max="8" width="10.54296875" customWidth="1"/>
-    <col min="9" max="9" width="14.08984375" customWidth="1"/>
-    <col min="10" max="10" width="15.81640625" customWidth="1"/>
-    <col min="11" max="11" width="11.54296875" customWidth="1"/>
-    <col min="12" max="12" width="11.36328125" customWidth="1"/>
-    <col min="13" max="13" width="13.6328125" customWidth="1"/>
+    <col min="2" max="2" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="15.90625" customWidth="1"/>
+    <col min="9" max="9" width="10.54296875" customWidth="1"/>
+    <col min="10" max="10" width="14.08984375" customWidth="1"/>
+    <col min="11" max="11" width="15.81640625" customWidth="1"/>
+    <col min="12" max="12" width="11.54296875" customWidth="1"/>
+    <col min="13" max="13" width="11.36328125" customWidth="1"/>
+    <col min="14" max="14" width="13.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>74</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>38</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>20</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>4</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>14</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>69</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>34</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>35</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>6</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>89</v>
+      </c>
+      <c r="E3">
+        <v>38</v>
+      </c>
+      <c r="F3">
+        <v>28</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <v>91</v>
+      </c>
+      <c r="J3">
+        <v>29</v>
+      </c>
+      <c r="K3">
+        <v>62</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3">
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A3" xr:uid="{F91F743A-E395-456E-9AA7-DFC2D0CBAC97}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>